<commit_message>
membuat sementara accepted rejected data dari pimpinan
</commit_message>
<xml_diff>
--- a/public/EmployeeData/LPSEKALSEL.xlsx
+++ b/public/EmployeeData/LPSEKALSEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thoriq\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40322663-C23E-4C62-86F3-E258F314358B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6540549-0C92-4569-9F2D-5B7E8F3546F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7E74542-3015-4755-8C13-23637B468A2B}"/>
   </bookViews>
@@ -144,7 +144,7 @@
     <t>Ballpoint 123</t>
   </si>
   <si>
-    <t>Banjarmasin</t>
+    <t>Banjarbaru</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>